<commit_message>
updates for FI curve analysis
</commit_message>
<xml_diff>
--- a/result_table_templates/MultiPulse_FIcurve.xlsx
+++ b/result_table_templates/MultiPulse_FIcurve.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregschwartz/matlab/DJ_schwartzlab/result_table_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6AAE4E-BF19-9746-9AE0-3DD38988B941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4B9C42-1AB6-7445-B6B0-A83D34D24CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23740" yWindow="600" windowWidth="22040" windowHeight="26260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,16 +70,16 @@
     <t>vector with how many trials for each injection size</t>
   </si>
   <si>
-    <t>FR_per_current_mean</t>
-  </si>
-  <si>
     <t>mean firing rate (Hz) for each current injection</t>
   </si>
   <si>
     <t>sem of firing rate (Hz) for each current injection</t>
   </si>
   <si>
-    <t>FR_per_current_sem</t>
+    <t>fr_per_current_mean</t>
+  </si>
+  <si>
+    <t>fr_per_current_sem</t>
   </si>
 </sst>
 </file>
@@ -437,7 +437,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -514,14 +514,14 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>16</v>
+      <c r="A7" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -532,7 +532,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>